<commit_message>
Fixed the last TestCase and expanded the Rest for the cost, margin, costMargin and costWithMargin - (Task #967)
---
Task #967: Add CostEquipmentWizard
</commit_message>
<xml_diff>
--- a/de.dlr.sc.virsat.model.extension.budget.cost.test/resources/ImportElementDefinitionTest.xlsx
+++ b/de.dlr.sc.virsat.model.extension.budget.cost.test/resources/ImportElementDefinitionTest.xlsx
@@ -8,21 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\VirtualSatellite4-Core\de.dlr.sc.virsat.model.extension.budget.cost.test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D33729E-E396-4942-9D39-3F998CB0C4C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A82C2301-D54C-42F3-874A-DBB6F91A9E70}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="108" windowWidth="20112" windowHeight="9528" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="108" windowWidth="20112" windowHeight="9528" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="1" r:id="rId1"/>
-    <sheet name="CostTypes" sheetId="8" r:id="rId2"/>
-    <sheet name="CostEquipments" sheetId="9" r:id="rId3"/>
+    <sheet name="CostEquipments" sheetId="10" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t xml:space="preserve"> Structural Element UUID</t>
   </si>
@@ -72,42 +71,15 @@
     <t>UUID</t>
   </si>
   <si>
-    <t>Interface Type</t>
-  </si>
-  <si>
-    <t>InterfaceEnd Name</t>
-  </si>
-  <si>
-    <t>Interface Type Name</t>
-  </si>
-  <si>
     <t>a2643ddb-e6a1-4015-9b80-be931f0c5a37</t>
   </si>
   <si>
-    <t>POW_IN</t>
-  </si>
-  <si>
-    <t>KILL</t>
-  </si>
-  <si>
     <t>9f8b18e1-f6a1-4cf6-bcb7-0d4a5f0a86de</t>
   </si>
   <si>
-    <t>POW_SOMETHING</t>
-  </si>
-  <si>
     <t>e13ad850-21d8-43d7-aa61-20a3f8d1749b</t>
   </si>
   <si>
-    <t>POW_OUT_C</t>
-  </si>
-  <si>
-    <t>HILL</t>
-  </si>
-  <si>
-    <t>POW_NEW</t>
-  </si>
-  <si>
     <t>supe_us</t>
   </si>
   <si>
@@ -120,10 +92,49 @@
     <t>BATTERY</t>
   </si>
   <si>
-    <t>VirSat IO Sheet for Cost Types</t>
-  </si>
-  <si>
-    <t>VirSat IO Sheet for CostEquipments</t>
+    <t>Cost Equipment Name</t>
+  </si>
+  <si>
+    <t>Cost Type</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>CostMaterial</t>
+  </si>
+  <si>
+    <t>CostPersonal</t>
+  </si>
+  <si>
+    <t>CostTest</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Personal</t>
+  </si>
+  <si>
+    <t>Cost Equipment FullQualifiedName</t>
+  </si>
+  <si>
+    <t>Margin %</t>
+  </si>
+  <si>
+    <t>Cost Margin</t>
+  </si>
+  <si>
+    <t>Cost with Margin</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>VirSat IO Sheet for Cost Equipments</t>
+  </si>
+  <si>
+    <t>This is an auto generated ICD Document of Virtual Satellite</t>
   </si>
 </sst>
 </file>
@@ -381,7 +392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -424,11 +435,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -445,6 +468,56 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>998221</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3185514" cy="906102"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79F522E9-3B89-4953-B710-C4B24DEF4165}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6339841" y="0"/>
+          <a:ext cx="3185514" cy="906102"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -819,7 +892,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C5" s="9"/>
     </row>
@@ -828,7 +901,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C6" s="2"/>
     </row>
@@ -837,7 +910,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C7" s="2"/>
     </row>
@@ -846,7 +919,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C8" s="2"/>
     </row>
@@ -911,81 +984,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C37"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="26.5546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="51.109375" style="2" customWidth="1"/>
-    <col min="4" max="256" width="9.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19"/>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-    </row>
-    <row r="2" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-    </row>
-    <row r="3" spans="1:3" ht="128.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="19"/>
-    </row>
-    <row r="4" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="24"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="A37:C37"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DDAEDD6-AF55-4F1E-9B5C-675526692FA1}">
+  <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D2"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -993,25 +996,39 @@
     <col min="1" max="1" width="26.5546875" style="3" customWidth="1"/>
     <col min="2" max="2" width="8.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="26.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5546875" style="2" customWidth="1"/>
-    <col min="5" max="256" width="9.109375" customWidth="1"/>
+    <col min="4" max="5" width="15.77734375" style="1" customWidth="1"/>
+    <col min="6" max="7" width="17.77734375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.77734375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="45.109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19"/>
+    <row r="1" spans="1:11" ht="72" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>37</v>
+      </c>
       <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-    </row>
-    <row r="2" spans="1:4" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+    </row>
+    <row r="2" spans="1:11" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
-    </row>
-    <row r="3" spans="1:4" ht="128.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+    </row>
+    <row r="3" spans="1:11" ht="128.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>12</v>
       </c>
@@ -1020,8 +1037,13 @@
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
-    </row>
-    <row r="4" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+    </row>
+    <row r="4" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
         <v>15</v>
       </c>
@@ -1029,69 +1051,518 @@
         <v>14</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
-        <v>19</v>
       </c>
       <c r="B5" s="8">
         <v>1</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="E5" s="32">
+        <v>1000</v>
+      </c>
+      <c r="F5" s="32">
+        <v>1100</v>
+      </c>
+      <c r="G5" s="32">
+        <v>100</v>
+      </c>
+      <c r="H5" s="32">
+        <v>10</v>
+      </c>
+      <c r="I5" s="31"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="E6" s="29">
+        <v>2000</v>
+      </c>
+      <c r="F6" s="29">
+        <v>2200</v>
+      </c>
+      <c r="G6" s="29">
+        <v>200</v>
+      </c>
+      <c r="H6" s="29">
+        <v>10</v>
+      </c>
+      <c r="I6" s="25"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="29">
+        <v>3000</v>
+      </c>
+      <c r="F7" s="29">
+        <v>3300</v>
+      </c>
+      <c r="G7" s="29">
+        <v>300</v>
+      </c>
+      <c r="H7" s="29">
+        <v>10</v>
+      </c>
+      <c r="I7" s="25"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="24"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
+      <c r="E8" s="29">
+        <v>4000</v>
+      </c>
+      <c r="F8" s="29">
+        <v>4400</v>
+      </c>
+      <c r="G8" s="29">
+        <v>400</v>
+      </c>
+      <c r="H8" s="29">
+        <v>10</v>
+      </c>
+      <c r="I8" s="25"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="30"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="30"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="30"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="30"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="30"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="30"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="30"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="30"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="30"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="30"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="30"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="30"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="30"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="30"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="30"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="30"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="30"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="30"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="24"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="30"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="25"/>
+      <c r="J27" s="24"/>
+      <c r="K27" s="24"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="30"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="24"/>
+      <c r="K28" s="24"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="30"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="24"/>
+      <c r="K29" s="24"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="30"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="25"/>
+      <c r="J30" s="24"/>
+      <c r="K30" s="24"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="30"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="25"/>
+      <c r="J31" s="24"/>
+      <c r="K31" s="24"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="30"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="29"/>
+      <c r="I32" s="25"/>
+      <c r="J32" s="24"/>
+      <c r="K32" s="24"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="30"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="25"/>
+      <c r="J33" s="24"/>
+      <c r="K33" s="24"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="30"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="25"/>
+      <c r="J34" s="24"/>
+      <c r="K34" s="24"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" s="30"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="29"/>
+      <c r="I35" s="25"/>
+      <c r="J35" s="24"/>
+      <c r="K35" s="24"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" s="30"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="29"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="29"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="29"/>
+      <c r="I36" s="25"/>
+      <c r="J36" s="24"/>
+      <c r="K36" s="24"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" s="28"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="26"/>
+      <c r="G37" s="26"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="25"/>
+      <c r="J37" s="24"/>
+      <c r="K37" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="B3:D3"/>
+  <mergeCells count="5">
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="B3:I3"/>
     <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>